<commit_message>
made database migrations in Django
</commit_message>
<xml_diff>
--- a/SLAPP_WIREFRAME1.xlsx
+++ b/SLAPP_WIREFRAME1.xlsx
@@ -4,11 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TableDesc" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha Geral" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Planilha Geral'!$A$1:$D$59</definedName>
+  </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -19,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="154">
   <si>
     <t>SLAP</t>
   </si>
@@ -253,13 +260,241 @@
   </si>
   <si>
     <t>Cliente.</t>
+  </si>
+  <si>
+    <t>Data:</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Itens técnicos:</t>
+  </si>
+  <si>
+    <t>Ajuste de tampos?</t>
+  </si>
+  <si>
+    <t>Pontos de elétrodomésticos?</t>
+  </si>
+  <si>
+    <t>Alinhamento de gavetas?</t>
+  </si>
+  <si>
+    <t>Passagem de gás?</t>
+  </si>
+  <si>
+    <t>Alinhamento de puxadores?</t>
+  </si>
+  <si>
+    <t>Luminárias?</t>
+  </si>
+  <si>
+    <t>Acabamento de recortes?</t>
+  </si>
+  <si>
+    <t>Passa-fios?</t>
+  </si>
+  <si>
+    <t>Acabamento interno?</t>
+  </si>
+  <si>
+    <t>Nivelamento?</t>
+  </si>
+  <si>
+    <t>Acabamento Externo?</t>
+  </si>
+  <si>
+    <t>Acesso aos pontos?</t>
+  </si>
+  <si>
+    <t>Meias Esquadrias?</t>
+  </si>
+  <si>
+    <t>Tonalidades?</t>
+  </si>
+  <si>
+    <t>Arremates e vistas?</t>
+  </si>
+  <si>
+    <t>Acabamento da fábrica?</t>
+  </si>
+  <si>
+    <t>Acabamentos de bordas?</t>
+  </si>
+  <si>
+    <t>Limpeza do ambiente?</t>
+  </si>
+  <si>
+    <t>Apresentação Pessoal:</t>
+  </si>
+  <si>
+    <t>Amortecedores portas e gavetas?</t>
+  </si>
+  <si>
+    <t>Recolhimento dos resíduos?</t>
+  </si>
+  <si>
+    <t>Fixação acessórios?</t>
+  </si>
+  <si>
+    <t>Vistas?</t>
+  </si>
+  <si>
+    <t>Funcionalidade de acessórios?</t>
+  </si>
+  <si>
+    <t>Montagem dos módulos?</t>
+  </si>
+  <si>
+    <t>Regulagem de aramados?</t>
+  </si>
+  <si>
+    <t>Roda-forros?</t>
+  </si>
+  <si>
+    <t>Regulagem de corrediças?</t>
+  </si>
+  <si>
+    <t>Riscos de lápis?</t>
+  </si>
+  <si>
+    <t>Regulagem de portas?</t>
+  </si>
+  <si>
+    <t>Capa de cantoneiras de fixação?</t>
+  </si>
+  <si>
+    <t>Tapa-furos?</t>
+  </si>
+  <si>
+    <t>Logomarca Todeschini?</t>
+  </si>
+  <si>
+    <t>Batentes silicone?</t>
+  </si>
+  <si>
+    <t>Nota do cliente para a montagem?</t>
+  </si>
+  <si>
+    <t>Antes da Montagem:</t>
+  </si>
+  <si>
+    <t>Esquadro fundos?</t>
+  </si>
+  <si>
+    <t>Reajuste entre o móvel e a parede?</t>
+  </si>
+  <si>
+    <t>Cabelos?</t>
+  </si>
+  <si>
+    <t>Esquadro piso e paredes?</t>
+  </si>
+  <si>
+    <t>Barba?</t>
+  </si>
+  <si>
+    <t>Forração do local da montagem?</t>
+  </si>
+  <si>
+    <t>Unhas?</t>
+  </si>
+  <si>
+    <t>Conferência de medidas?</t>
+  </si>
+  <si>
+    <t>Uniforme?</t>
+  </si>
+  <si>
+    <t>Conferência de material?</t>
+  </si>
+  <si>
+    <t>Retorno à loja:</t>
+  </si>
+  <si>
+    <t>Higiene Pessoal?</t>
+  </si>
+  <si>
+    <t>Plantas Elétricas e Hidráulicas?</t>
+  </si>
+  <si>
+    <t>Comportamento na casa cliente?</t>
+  </si>
+  <si>
+    <t>Informou o tempo ao cliente?</t>
+  </si>
+  <si>
+    <t>Durante a montagem:</t>
+  </si>
+  <si>
+    <t>Após a montagem:</t>
+  </si>
+  <si>
+    <t>Garantiu a qualidade da marca?</t>
+  </si>
+  <si>
+    <t>Fez a limpeza do local?</t>
+  </si>
+  <si>
+    <t>Cuidou da limpeza do local?</t>
+  </si>
+  <si>
+    <t>Deu orientações ao cliente?</t>
+  </si>
+  <si>
+    <t>Repassou informações à loja (vendedor, projetista, supervisor de montagem, gerente)?</t>
+  </si>
+  <si>
+    <t>Nota Final da Montagem/Montador</t>
+  </si>
+  <si>
+    <t>Legenda</t>
+  </si>
+  <si>
+    <t>Ruim</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bom </t>
+  </si>
+  <si>
+    <t>Bom</t>
+  </si>
+  <si>
+    <t>Ótimo</t>
+  </si>
+  <si>
+    <t>Obs: O Check-list deve ser preenchido pelo responsável do setor de montagem da respectiva loja,</t>
+  </si>
+  <si>
+    <t>sempre mediante análise e/ou auditoria do processo.</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>Instalación de Muebles</t>
+  </si>
+  <si>
+    <t>Cliente:</t>
+  </si>
+  <si>
+    <t>Proveedor:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compañía/Supervisor ** : </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -340,8 +575,80 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -372,8 +679,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -381,8 +706,75 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -474,8 +866,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,8 +898,76 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="91"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="91" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="91" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="91" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="91" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="91" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="91" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="91" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="91" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="91" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="4" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="4" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="4" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="91" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="19" fillId="7" borderId="0" xfId="91" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="91" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="91" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="91" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -549,6 +1019,14 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -589,10 +1067,172 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="91"/>
+    <cellStyle name="Percent 2" xfId="92"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Planilha Geral"/>
+      <sheetName val="Gráficos"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="10">
+          <cell r="L10" t="str">
+            <v>ruim:</v>
+          </cell>
+          <cell r="M10">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="L11" t="str">
+            <v>regular:</v>
+          </cell>
+          <cell r="M11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="L12" t="str">
+            <v>bom:</v>
+          </cell>
+          <cell r="M12">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="L13" t="str">
+            <v>ótimo:</v>
+          </cell>
+          <cell r="M13">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="L18" t="str">
+            <v>ruim:</v>
+          </cell>
+          <cell r="M18">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="L19" t="str">
+            <v>regular:</v>
+          </cell>
+          <cell r="M19">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="L20" t="str">
+            <v>bom:</v>
+          </cell>
+          <cell r="M20">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="L21" t="str">
+            <v>ótimo:</v>
+          </cell>
+          <cell r="M21">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="L26" t="str">
+            <v>ruim:</v>
+          </cell>
+          <cell r="M26">
+            <v>0</v>
+          </cell>
+          <cell r="N26" t="str">
+            <v>ruim:</v>
+          </cell>
+          <cell r="O26">
+            <v>0</v>
+          </cell>
+          <cell r="P26" t="str">
+            <v>ruim:</v>
+          </cell>
+          <cell r="Q26">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="L27" t="str">
+            <v>regular:</v>
+          </cell>
+          <cell r="M27">
+            <v>0</v>
+          </cell>
+          <cell r="N27" t="str">
+            <v>regular:</v>
+          </cell>
+          <cell r="O27">
+            <v>0</v>
+          </cell>
+          <cell r="P27" t="str">
+            <v>regular:</v>
+          </cell>
+          <cell r="Q27">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="L28" t="str">
+            <v>bom:</v>
+          </cell>
+          <cell r="M28">
+            <v>0</v>
+          </cell>
+          <cell r="N28" t="str">
+            <v>bom:</v>
+          </cell>
+          <cell r="O28">
+            <v>0</v>
+          </cell>
+          <cell r="P28" t="str">
+            <v>bom:</v>
+          </cell>
+          <cell r="Q28">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="L29" t="str">
+            <v>ótimo:</v>
+          </cell>
+          <cell r="M29">
+            <v>0</v>
+          </cell>
+          <cell r="N29" t="str">
+            <v>ótimo:</v>
+          </cell>
+          <cell r="O29">
+            <v>0</v>
+          </cell>
+          <cell r="P29" t="str">
+            <v>ótimo:</v>
+          </cell>
+          <cell r="Q29">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -919,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1649,4 +2289,620 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="32.5" style="17" customWidth="1"/>
+    <col min="4" max="4" width="8" style="17" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="17"/>
+    <col min="6" max="6" width="28.6640625" style="17" customWidth="1"/>
+    <col min="7" max="9" width="20.6640625" style="17" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9">
+      <c r="A2" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="47"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="19"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="46"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="20"/>
+      <c r="B8" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="A9" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="F9" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" s="36">
+        <v>0</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="I9" s="36">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="36">
+        <v>0.26</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" s="36">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G11" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="I11" s="37">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="38">
+        <v>0.76</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="I12" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="G14" s="40"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="41"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" s="21"/>
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" ht="18">
+      <c r="A16" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="43">
+        <f>COUNTIF($B$8:$D$45,TRUE)/(COUNTIF($B$8:$D$45,FALSE)+COUNTIF($B$8:$D$45,TRUE))</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18">
+      <c r="A17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="G17" s="44" t="str">
+        <f>IF(G16&lt;25%,"Ruim",IF(G16&lt;50%,"Regular",IF(G16&lt;75%,"Bom","Otimo")))</f>
+        <v>Bom</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="21"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="23"/>
+      <c r="C30" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="23"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D36" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="27"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="20"/>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="B38" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="23"/>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B41" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D41" s="24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="21"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="B43" s="39"/>
+      <c r="D43" s="35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="20"/>
+      <c r="D44" s="23"/>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B45" s="30"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>